<commit_message>
Update 1.3.2: Paginated loader and  2 update reference-books
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта материалов.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта материалов.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C867E3C8-EDBD-4149-A90D-B60CF9528F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9572AE45-D5AC-418E-AA7C-98B6E3899B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Материалы" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -448,7 +448,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>